<commit_message>
Remove AI disclaimer and fix OS calculation to use proper Kaplan-Meier method
</commit_message>
<xml_diff>
--- a/Calcoli_RDD_2025-1.xlsx
+++ b/Calcoli_RDD_2025-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta.stanzani\Documents\RRD_2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russelllewis/JACIE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07670A47-3576-4046-9296-2F9AA6D9B2DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE8D660-D475-0249-9A1D-54752E0C6829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{703575B0-2B93-4ABD-A5A8-F4C311633005}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{703575B0-2B93-4ABD-A5A8-F4C311633005}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="254">
   <si>
     <t>N.</t>
   </si>
@@ -786,6 +786,18 @@
   </si>
   <si>
     <t>dead for infection with GVHD</t>
+  </si>
+  <si>
+    <t>death_type</t>
+  </si>
+  <si>
+    <t>RRM</t>
+  </si>
+  <si>
+    <t>TRM</t>
+  </si>
+  <si>
+    <t>NRM</t>
   </si>
 </sst>
 </file>
@@ -876,7 +888,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -944,11 +956,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1013,9 +1036,12 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1031,9 +1057,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1071,7 +1097,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1177,7 +1203,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1319,7 +1345,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1327,43 +1353,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D83052-2E0F-4E3D-80E3-9D814D130B0D}">
-  <dimension ref="A1:AF48"/>
+  <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" customWidth="1"/>
-    <col min="26" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="42" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="15.5" customWidth="1"/>
+    <col min="20" max="20" width="36.5" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" customWidth="1"/>
+    <col min="22" max="22" width="6.5" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.5" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" customWidth="1"/>
+    <col min="26" max="27" width="10.6640625" customWidth="1"/>
+    <col min="28" max="28" width="4.6640625" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25" customWidth="1"/>
+    <col min="31" max="31" width="0.1640625" customWidth="1"/>
+    <col min="32" max="32" width="5.5" customWidth="1"/>
+    <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,8 +1489,11 @@
       <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="22" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1551,7 +1583,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1645,7 +1677,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1735,7 +1767,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1824,8 +1856,11 @@
       <c r="AF5" s="9">
         <v>223</v>
       </c>
+      <c r="AG5" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1914,8 +1949,11 @@
       <c r="AF6" s="9">
         <v>144</v>
       </c>
+      <c r="AG6" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2004,8 +2042,11 @@
       <c r="AF7" s="9">
         <v>24</v>
       </c>
+      <c r="AG7" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2098,8 +2139,11 @@
       <c r="AF8" s="9">
         <v>103</v>
       </c>
+      <c r="AG8" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2188,8 +2232,11 @@
       <c r="AF9" s="9">
         <v>162</v>
       </c>
+      <c r="AG9" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2283,7 +2330,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2372,8 +2419,11 @@
       <c r="AF11" s="9">
         <v>243</v>
       </c>
+      <c r="AG11" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2463,7 +2513,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2552,8 +2602,11 @@
       <c r="AF13" s="9">
         <v>238</v>
       </c>
+      <c r="AG13" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2643,7 +2696,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2733,7 +2786,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2823,7 +2876,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2912,8 +2965,11 @@
       <c r="AF17" s="9">
         <v>428</v>
       </c>
+      <c r="AG17" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3007,7 +3063,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -3101,7 +3157,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -3195,7 +3251,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -3293,7 +3349,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -3389,7 +3445,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -3483,7 +3539,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -3573,7 +3629,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -3667,7 +3723,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -3761,7 +3817,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -3859,7 +3915,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -3949,7 +4005,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -4039,7 +4095,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -4129,7 +4185,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -4219,7 +4275,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -4317,7 +4373,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -4407,7 +4463,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -4505,7 +4561,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -4595,7 +4651,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -4689,7 +4745,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -4785,7 +4841,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -4875,7 +4931,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -4965,7 +5021,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -5063,7 +5119,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -5153,7 +5209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -5241,7 +5297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -5324,8 +5380,11 @@
       <c r="AF43" s="9">
         <v>30</v>
       </c>
+      <c r="AG43" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="44" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -5413,7 +5472,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -5501,7 +5560,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -5589,7 +5648,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -5677,7 +5736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>

</xml_diff>